<commit_message>
classic ML algos for OS data
</commit_message>
<xml_diff>
--- a/Results/Classic_ML_Results.xlsx
+++ b/Results/Classic_ML_Results.xlsx
@@ -13,9 +13,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="22">
   <si>
-    <t>Classic ML algorithms on features</t>
+    <t>Classic ML algorithms on features - Normal Data</t>
   </si>
   <si>
     <t>Pos_neg_ratio</t>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 50:50</t>
+  </si>
+  <si>
+    <t>Classic ML algorithms on features - OverSampled Data</t>
   </si>
 </sst>
 </file>
@@ -1310,6 +1313,1016 @@
       <c r="U67" s="16"/>
       <c r="V67" s="16"/>
     </row>
+    <row r="70" ht="19.5">
+      <c r="A70" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
+      <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73">
+        <v>1359.0</v>
+      </c>
+      <c r="D73">
+        <v>339.0</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" s="7">
+        <v>81.9</v>
+      </c>
+      <c r="H73" s="7">
+        <v>98.0</v>
+      </c>
+      <c r="I73" s="7">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="5"/>
+      <c r="B74" s="6"/>
+      <c r="E74" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G74" s="8">
+        <v>87.0</v>
+      </c>
+      <c r="H74" s="9">
+        <v>98.9</v>
+      </c>
+      <c r="I74" s="9">
+        <v>63.6</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="5"/>
+      <c r="B75" s="6"/>
+      <c r="E75" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G75" s="7">
+        <v>86.7</v>
+      </c>
+      <c r="H75" s="7">
+        <v>98.3</v>
+      </c>
+      <c r="I75" s="7">
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="5"/>
+      <c r="B76" s="6"/>
+      <c r="E76" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G76" s="10">
+        <v>76.6</v>
+      </c>
+      <c r="H76" s="10">
+        <v>83.4</v>
+      </c>
+      <c r="I76" s="10">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="5"/>
+      <c r="B77" s="6"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78">
+        <v>1186.0</v>
+      </c>
+      <c r="D78">
+        <v>512.0</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" t="s">
+        <v>12</v>
+      </c>
+      <c r="G78" s="7">
+        <v>81.8</v>
+      </c>
+      <c r="H78" s="7">
+        <v>98.0</v>
+      </c>
+      <c r="I78" s="7">
+        <v>85.4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="5"/>
+      <c r="B79" s="6"/>
+      <c r="E79" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G79" s="7">
+        <v>86.1</v>
+      </c>
+      <c r="H79" s="7">
+        <v>98.6</v>
+      </c>
+      <c r="I79" s="7">
+        <v>65.7</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="5"/>
+      <c r="B80" s="6"/>
+      <c r="E80" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" s="9">
+        <v>86.0</v>
+      </c>
+      <c r="H80" s="9">
+        <v>98.0</v>
+      </c>
+      <c r="I80" s="9">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="5"/>
+      <c r="B81" s="6"/>
+      <c r="E81" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G81" s="11">
+        <v>76.0</v>
+      </c>
+      <c r="H81" s="11">
+        <v>82.9</v>
+      </c>
+      <c r="I81" s="11">
+        <v>52.6</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C83">
+        <v>1019.0</v>
+      </c>
+      <c r="D83">
+        <v>679.0</v>
+      </c>
+      <c r="E83" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="7">
+        <v>81.86</v>
+      </c>
+      <c r="H83" s="7">
+        <v>98.2</v>
+      </c>
+      <c r="I83" s="7">
+        <v>86.1</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="12"/>
+      <c r="E84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" s="7">
+        <v>85.7</v>
+      </c>
+      <c r="H84" s="7">
+        <v>98.6</v>
+      </c>
+      <c r="I84" s="7">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="5"/>
+      <c r="B85" s="12"/>
+      <c r="E85" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" s="9">
+        <v>85.4</v>
+      </c>
+      <c r="H85" s="9">
+        <v>97.5</v>
+      </c>
+      <c r="I85" s="9">
+        <v>64.8</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="5"/>
+      <c r="B86" s="12"/>
+      <c r="E86" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G86" s="11">
+        <v>75.4</v>
+      </c>
+      <c r="H86" s="11">
+        <v>82.8</v>
+      </c>
+      <c r="I86" s="11">
+        <v>54.9</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="5"/>
+      <c r="B87" s="12"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="14"/>
+      <c r="B88" s="15"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>1551.0</v>
+      </c>
+      <c r="D89">
+        <v>389.0</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="9">
+        <v>74.04</v>
+      </c>
+      <c r="H89" s="9">
+        <v>78.1</v>
+      </c>
+      <c r="I89" s="9">
+        <v>35.8</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="5"/>
+      <c r="E90" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G90" s="11">
+        <v>82.79</v>
+      </c>
+      <c r="H90" s="11">
+        <v>82.3</v>
+      </c>
+      <c r="I90" s="11">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="5"/>
+      <c r="E91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" s="9">
+        <v>81.8</v>
+      </c>
+      <c r="H91" s="9">
+        <v>81.2</v>
+      </c>
+      <c r="I91" s="9">
+        <v>18.2</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="5"/>
+      <c r="E92" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G92" s="9">
+        <v>71.61</v>
+      </c>
+      <c r="H92" s="9">
+        <v>81.5</v>
+      </c>
+      <c r="I92" s="9">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="5"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
+    </row>
+    <row r="94">
+      <c r="A94" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B94" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94">
+        <v>1356.0</v>
+      </c>
+      <c r="D94">
+        <v>584.0</v>
+      </c>
+      <c r="E94" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="9">
+        <v>73.67</v>
+      </c>
+      <c r="H94" s="9">
+        <v>77.7</v>
+      </c>
+      <c r="I94" s="9">
+        <v>36.2</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="5"/>
+      <c r="E95" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G95" s="11">
+        <v>81.88</v>
+      </c>
+      <c r="H95" s="11">
+        <v>82.0</v>
+      </c>
+      <c r="I95" s="11">
+        <v>18.3</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="5"/>
+      <c r="E96" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="9">
+        <v>81.0</v>
+      </c>
+      <c r="H96" s="9">
+        <v>80.6</v>
+      </c>
+      <c r="I96" s="9">
+        <v>17.9</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="5"/>
+      <c r="E97" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G97" s="9">
+        <v>71.21</v>
+      </c>
+      <c r="H97" s="9">
+        <v>81.1</v>
+      </c>
+      <c r="I97" s="9">
+        <v>52.7</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="5"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99">
+        <v>1165.0</v>
+      </c>
+      <c r="D99">
+        <v>775.0</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" t="s">
+        <v>12</v>
+      </c>
+      <c r="G99" s="9">
+        <v>73.69</v>
+      </c>
+      <c r="H99" s="9">
+        <v>78.0</v>
+      </c>
+      <c r="I99" s="9">
+        <v>36.3</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" t="s">
+        <v>18</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G100" s="11">
+        <v>81.0</v>
+      </c>
+      <c r="H100" s="11">
+        <v>81.6</v>
+      </c>
+      <c r="I100" s="11">
+        <v>20.3</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="5"/>
+      <c r="E101" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G101" s="9">
+        <v>80.43</v>
+      </c>
+      <c r="H101" s="9">
+        <v>80.7</v>
+      </c>
+      <c r="I101" s="9">
+        <v>20.1</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="5"/>
+      <c r="E102" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G102" s="9">
+        <v>71.42</v>
+      </c>
+      <c r="H102" s="9">
+        <v>81.7</v>
+      </c>
+      <c r="I102" s="9">
+        <v>52.4</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="5"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+    </row>
+    <row r="104">
+      <c r="A104" s="14"/>
+      <c r="B104" s="16"/>
+      <c r="C104" s="16"/>
+      <c r="D104" s="16"/>
+      <c r="E104" s="16"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
+    </row>
+    <row r="105">
+      <c r="A105" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B105" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>1810.0</v>
+      </c>
+      <c r="D105">
+        <v>454.0</v>
+      </c>
+      <c r="E105" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" s="9">
+        <v>73.18</v>
+      </c>
+      <c r="H105" s="9">
+        <v>75.6</v>
+      </c>
+      <c r="I105" s="9">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="E106" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G106" s="11">
+        <v>84.17</v>
+      </c>
+      <c r="H106" s="11">
+        <v>82.3</v>
+      </c>
+      <c r="I106" s="11">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="E107" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G107" s="9">
+        <v>82.9</v>
+      </c>
+      <c r="H107" s="9">
+        <v>81.5</v>
+      </c>
+      <c r="I107" s="9">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="E108" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G108" s="7">
+        <v>69.33</v>
+      </c>
+      <c r="H108" s="7">
+        <v>82.8</v>
+      </c>
+      <c r="I108" s="7">
+        <v>51.9</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="E109" s="7"/>
+    </row>
+    <row r="110">
+      <c r="A110" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B110" t="s">
+        <v>16</v>
+      </c>
+      <c r="C110">
+        <v>1583.0</v>
+      </c>
+      <c r="D110">
+        <v>681.0</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F110" t="s">
+        <v>19</v>
+      </c>
+      <c r="G110" s="7">
+        <v>73.01</v>
+      </c>
+      <c r="H110" s="7">
+        <v>75.2</v>
+      </c>
+      <c r="I110" s="7">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="E111" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G111" s="10">
+        <v>83.08</v>
+      </c>
+      <c r="H111" s="10">
+        <v>81.6</v>
+      </c>
+      <c r="I111" s="10">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="E112" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G112" s="7">
+        <v>82.18</v>
+      </c>
+      <c r="H112" s="9">
+        <v>80.6</v>
+      </c>
+      <c r="I112" s="7">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="E113" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G113" s="9">
+        <v>68.96</v>
+      </c>
+      <c r="H113" s="9">
+        <v>82.1</v>
+      </c>
+      <c r="I113" s="9">
+        <v>51.6</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B115" t="s">
+        <v>17</v>
+      </c>
+      <c r="C115">
+        <v>1357.0</v>
+      </c>
+      <c r="D115">
+        <v>907.0</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" t="s">
+        <v>19</v>
+      </c>
+      <c r="G115" s="7">
+        <v>73.54</v>
+      </c>
+      <c r="H115" s="7">
+        <v>75.7</v>
+      </c>
+      <c r="I115" s="7">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="E116" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G116" s="10">
+        <v>82.98</v>
+      </c>
+      <c r="H116" s="10">
+        <v>81.6</v>
+      </c>
+      <c r="I116" s="10">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="E117" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G117" s="9">
+        <v>81.7</v>
+      </c>
+      <c r="H117" s="9">
+        <v>80.2</v>
+      </c>
+      <c r="I117" s="9">
+        <v>15.7</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="E118" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G118" s="7">
+        <v>69.22</v>
+      </c>
+      <c r="H118" s="7">
+        <v>82.1</v>
+      </c>
+      <c r="I118" s="7">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="E119" s="7"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="16"/>
+      <c r="B120" s="16"/>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B121" t="s">
+        <v>10</v>
+      </c>
+      <c r="C121">
+        <v>2174.0</v>
+      </c>
+      <c r="D121">
+        <v>544.0</v>
+      </c>
+      <c r="E121" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" t="s">
+        <v>19</v>
+      </c>
+      <c r="G121" s="7">
+        <v>74.5</v>
+      </c>
+      <c r="H121" s="7">
+        <v>71.4</v>
+      </c>
+      <c r="I121" s="7">
+        <v>22.4</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="E122" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G122" s="10">
+        <v>85.24</v>
+      </c>
+      <c r="H122" s="10">
+        <v>80.7</v>
+      </c>
+      <c r="I122" s="10">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="E123" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G123" s="7">
+        <v>83.84</v>
+      </c>
+      <c r="H123" s="7">
+        <v>80.1</v>
+      </c>
+      <c r="I123" s="7">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="E124" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G124" s="9">
+        <v>66.17</v>
+      </c>
+      <c r="H124" s="9">
+        <v>81.9</v>
+      </c>
+      <c r="I124" s="9">
+        <v>49.4</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C126">
+        <v>1901.0</v>
+      </c>
+      <c r="D126">
+        <v>817.0</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F126" t="s">
+        <v>19</v>
+      </c>
+      <c r="G126" s="7">
+        <v>74.34</v>
+      </c>
+      <c r="H126" s="7">
+        <v>70.9</v>
+      </c>
+      <c r="I126" s="7">
+        <v>22.3</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="E127" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G127" s="10">
+        <v>84.59</v>
+      </c>
+      <c r="H127" s="10">
+        <v>79.8</v>
+      </c>
+      <c r="I127" s="10">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="E128" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G128" s="7">
+        <v>83.61</v>
+      </c>
+      <c r="H128" s="7">
+        <v>79.8</v>
+      </c>
+      <c r="I128" s="7">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="E129" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G129" s="7">
+        <v>66.29</v>
+      </c>
+      <c r="H129" s="7">
+        <v>81.9</v>
+      </c>
+      <c r="I129" s="7">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B131" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131">
+        <v>1630.0</v>
+      </c>
+      <c r="D131">
+        <v>1088.0</v>
+      </c>
+      <c r="E131" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" t="s">
+        <v>19</v>
+      </c>
+      <c r="G131" s="7">
+        <v>73.99</v>
+      </c>
+      <c r="H131" s="7">
+        <v>69.5</v>
+      </c>
+      <c r="I131" s="7">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="E132" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G132" s="10">
+        <v>84.1</v>
+      </c>
+      <c r="H132" s="10">
+        <v>78.9</v>
+      </c>
+      <c r="I132" s="10">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="E133" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G133" s="7">
+        <v>82.8</v>
+      </c>
+      <c r="H133" s="7">
+        <v>78.8</v>
+      </c>
+      <c r="I133" s="7">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="E134" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G134" s="7">
+        <v>66.9</v>
+      </c>
+      <c r="H134" s="7">
+        <v>81.2</v>
+      </c>
+      <c r="I134" s="7">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="E135" s="18"/>
+    </row>
+    <row r="136">
+      <c r="A136" s="16"/>
+      <c r="B136" s="16"/>
+      <c r="C136" s="16"/>
+      <c r="D136" s="16"/>
+      <c r="E136" s="16"/>
+      <c r="F136" s="16"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="16"/>
+      <c r="I136" s="16"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>